<commit_message>
Curso de PHP y MySql [15.- Operadores matemáticos (Parte 2)]
Video:
https://youtu.be/g619ZLbBPFU
</commit_message>
<xml_diff>
--- a/Operadores mateaticos.xlsx
+++ b/Operadores mateaticos.xlsx
@@ -97,7 +97,7 @@
     <t xml:space="preserve">$a ** $b</t>
   </si>
   <si>
-    <t xml:space="preserve">Exponenciación</t>
+    <t xml:space="preserve">Exponencial</t>
   </si>
   <si>
     <t xml:space="preserve">Resultado de elevar $a a la potencia $bésima.</t>
@@ -295,8 +295,8 @@
   </sheetPr>
   <dimension ref="B1:D9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="280" zoomScaleNormal="280" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -396,7 +396,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="2" t="s">
         <v>24</v>
       </c>

</xml_diff>